<commit_message>
Updating excel document with table 1 and 2
</commit_message>
<xml_diff>
--- a/John_Tables.xlsx
+++ b/John_Tables.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fisher/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e655411\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ED23CB2-79CE-9E47-B62D-35C5E5916B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACAC6CD-D711-48D9-93AE-C56031864DC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16300" xr2:uid="{6DA41870-87E3-864C-BE65-46ADE84C5C34}"/>
+    <workbookView xWindow="7950" yWindow="126" windowWidth="13398" windowHeight="11430" xr2:uid="{6DA41870-87E3-864C-BE65-46ADE84C5C34}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
     <sheet name="Table2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t>Table 2. Hazard of death 20 years after baseline by baseline alcohol consumption.</t>
   </si>
@@ -91,18 +91,9 @@
     <t>Characteristic</t>
   </si>
   <si>
-    <t>Total n (column %)</t>
-  </si>
-  <si>
-    <t>Person-years of follow-up, n (%)</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Total person-years of follow-up</t>
-  </si>
-  <si>
     <t>Demographic variables</t>
   </si>
   <si>
@@ -218,6 +209,84 @@
   </si>
   <si>
     <t>28 (30.1)</t>
+  </si>
+  <si>
+    <t>41.72 (12.88)</t>
+  </si>
+  <si>
+    <t>Gender, n(%)</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>2006 (49.8)</t>
+  </si>
+  <si>
+    <t>2022 (50.2)</t>
+  </si>
+  <si>
+    <t>1927 (47.8)</t>
+  </si>
+  <si>
+    <t>1471 (36.5)</t>
+  </si>
+  <si>
+    <t>630 (15.6)</t>
+  </si>
+  <si>
+    <t>676 (16.8)</t>
+  </si>
+  <si>
+    <t>920 (22.8)</t>
+  </si>
+  <si>
+    <t>839 (20.8)</t>
+  </si>
+  <si>
+    <t>485 (12.0)</t>
+  </si>
+  <si>
+    <t>1108 (27.5)</t>
+  </si>
+  <si>
+    <t>675 (16.8)</t>
+  </si>
+  <si>
+    <t>1926 (47.8)</t>
+  </si>
+  <si>
+    <t>1427 (35.4)</t>
+  </si>
+  <si>
+    <t>447 (11.1)</t>
+  </si>
+  <si>
+    <t>2203 (54.7)</t>
+  </si>
+  <si>
+    <t>674 (16.7)</t>
+  </si>
+  <si>
+    <t>383 (9.5)</t>
+  </si>
+  <si>
+    <t>228 (5.7)</t>
+  </si>
+  <si>
+    <t>93 (2.3)</t>
+  </si>
+  <si>
+    <t>20.66 (3.97)</t>
+  </si>
+  <si>
+    <t>Total person-years of follow-up, mean (SD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Person-years of follow-up</t>
   </si>
 </sst>
 </file>
@@ -680,6 +749,105 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -700,105 +868,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1114,267 +1183,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34E9464-3AEF-074E-A273-00B1548652C2}">
-  <dimension ref="B2:E31"/>
+  <dimension ref="B2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="5" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="4.6484375" customWidth="1"/>
+    <col min="3" max="3" width="31.1484375" customWidth="1"/>
+    <col min="4" max="5" width="17.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+    <row r="2" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65"/>
+    <row r="3" spans="2:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="2:5" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="2:5" ht="23.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="2:5" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="25" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="2:5" ht="27.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:5" ht="17.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B7" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B8" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="38"/>
-    </row>
-    <row r="7" spans="2:5" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B10" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B11" s="17"/>
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="38"/>
-    </row>
-    <row r="8" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="D11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B12" s="16"/>
+      <c r="C12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="39"/>
-    </row>
-    <row r="9" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B14" s="17"/>
+      <c r="C14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="38"/>
-    </row>
-    <row r="10" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
-      <c r="C10" s="20" t="s">
+      <c r="D14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B15" s="17"/>
+      <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="38"/>
-    </row>
-    <row r="11" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
+      <c r="D15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B16" s="16"/>
+      <c r="C16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="38"/>
-    </row>
-    <row r="12" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
-      <c r="C12" s="20" t="s">
+      <c r="D16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="38"/>
-    </row>
-    <row r="13" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="20" t="s">
+      <c r="C17" s="22"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B18" s="17"/>
+      <c r="C18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="38"/>
-    </row>
-    <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
-      <c r="C14" s="20" t="s">
+      <c r="D18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B19" s="17"/>
+      <c r="C19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="38"/>
-    </row>
-    <row r="15" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="D19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B20" s="17"/>
+      <c r="C20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="38"/>
-    </row>
-    <row r="16" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="20" t="s">
+      <c r="D20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B21" s="17"/>
+      <c r="C21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="38"/>
-    </row>
-    <row r="17" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
-      <c r="C17" s="20" t="s">
+      <c r="D21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B22" s="16"/>
+      <c r="C22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="38"/>
-    </row>
-    <row r="18" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
-      <c r="C18" s="20" t="s">
+      <c r="D22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B23" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="38"/>
-    </row>
-    <row r="19" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
-      <c r="C19" s="20" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B24" s="17"/>
+      <c r="C24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="38"/>
-    </row>
-    <row r="20" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
-      <c r="C20" s="20" t="s">
+      <c r="D24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B25" s="17"/>
+      <c r="C25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="38"/>
-    </row>
-    <row r="21" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="37" t="s">
+      <c r="D25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B26" s="16"/>
+      <c r="C26" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="38"/>
-    </row>
-    <row r="22" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="41"/>
-      <c r="C22" s="20" t="s">
+      <c r="D26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B27" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="38"/>
-    </row>
-    <row r="23" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="41"/>
-      <c r="C23" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="38"/>
-    </row>
-    <row r="24" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
-      <c r="C24" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="38"/>
-    </row>
-    <row r="25" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="38"/>
-    </row>
-    <row r="26" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="41"/>
-      <c r="C26" s="20" t="s">
+      <c r="C27" s="22"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B28" s="17"/>
+      <c r="C28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="38"/>
-    </row>
-    <row r="27" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
-      <c r="C27" s="26" t="s">
+      <c r="D28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B29" s="17"/>
+      <c r="C29" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="38"/>
-    </row>
-    <row r="28" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="41"/>
-      <c r="C28" s="20" t="s">
+      <c r="D29" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B30" s="17"/>
+      <c r="C30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="38"/>
-    </row>
-    <row r="29" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="41"/>
-      <c r="C29" s="20" t="s">
+      <c r="D30" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B31" s="17"/>
+      <c r="C31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="38"/>
-    </row>
-    <row r="30" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="41"/>
-      <c r="C30" s="20" t="s">
+      <c r="D31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B32" s="17"/>
+      <c r="C32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="38"/>
-    </row>
-    <row r="31" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
-      <c r="C31" s="43" t="s">
+      <c r="D32" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B33" s="18"/>
+      <c r="C33" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="44"/>
+      <c r="D33" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B4:C4"/>
+  <mergeCells count="12">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1388,56 +1516,56 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="5" max="7" width="17.6640625" customWidth="1"/>
+    <col min="5" max="7" width="17.6484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:9" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="2" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65"/>
+    <row r="3" spans="2:9" ht="26.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="44" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+    <row r="5" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B5" s="43"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1445,7 +1573,7 @@
         <v>447</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
@@ -1459,7 +1587,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1467,21 +1595,21 @@
         <v>2203</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1489,21 +1617,21 @@
         <v>674</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1511,21 +1639,21 @@
         <v>383</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1533,21 +1661,21 @@
         <v>228</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1555,41 +1683,41 @@
         <v>93</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+    <row r="12" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B12" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:9" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="2:9" ht="26.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated Table 1 person-time column
Made formatting changes and added person time data (mean sd)
</commit_message>
<xml_diff>
--- a/John_Tables.xlsx
+++ b/John_Tables.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e655411\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catherine Cortez\Desktop\EPI 207\EPI 207_GitKraken\Epidem207_JohnB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACAC6CD-D711-48D9-93AE-C56031864DC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411B4C35-F591-409F-A2F6-6A9E568F3E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7950" yWindow="126" windowWidth="13398" windowHeight="11430" xr2:uid="{6DA41870-87E3-864C-BE65-46ADE84C5C34}"/>
+    <workbookView xWindow="2263" yWindow="2263" windowWidth="16457" windowHeight="9548" xr2:uid="{6DA41870-87E3-864C-BE65-46ADE84C5C34}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table1" sheetId="4" r:id="rId1"/>
+    <sheet name="Table1 (archived)" sheetId="1" r:id="rId2"/>
+    <sheet name="Table2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="107">
   <si>
     <t>Table 2. Hazard of death 20 years after baseline by baseline alcohol consumption.</t>
   </si>
@@ -287,13 +288,83 @@
   </si>
   <si>
     <t>Person-years of follow-up</t>
+  </si>
+  <si>
+    <t>Total n (column %)</t>
+  </si>
+  <si>
+    <t>Person-years of follow-up
+Mean (SD)</t>
+  </si>
+  <si>
+    <t>4028 (100)</t>
+  </si>
+  <si>
+    <t>20.66 (4.0)</t>
+  </si>
+  <si>
+    <t>41.72 (12.9)</t>
+  </si>
+  <si>
+    <t>21.0 (3.4)</t>
+  </si>
+  <si>
+    <t>20.1 (4.7)</t>
+  </si>
+  <si>
+    <t>21.2 (3.0)</t>
+  </si>
+  <si>
+    <t>21.2 (3.2)</t>
+  </si>
+  <si>
+    <t>20.9 (3.6)</t>
+  </si>
+  <si>
+    <t>21.3 (2.9)</t>
+  </si>
+  <si>
+    <t>20.5 (4.3)</t>
+  </si>
+  <si>
+    <t>20.8 (3.6)</t>
+  </si>
+  <si>
+    <t>20.0 (4.7)</t>
+  </si>
+  <si>
+    <t>20.7 (3.9)</t>
+  </si>
+  <si>
+    <t>19.3 (5.3)</t>
+  </si>
+  <si>
+    <t>19.3 (5.4)</t>
+  </si>
+  <si>
+    <t>Low to Moderate  (AUDIT-C=1-3)</t>
+  </si>
+  <si>
+    <t>21.0 (3.5)</t>
+  </si>
+  <si>
+    <t>20.9 (3.5)</t>
+  </si>
+  <si>
+    <t>20.3 (4.6)</t>
+  </si>
+  <si>
+    <t>18.9 (5.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Abbreviations: AUDIT-C, Alcohol Use Disorders Identification Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -327,6 +398,48 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -336,7 +449,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -728,11 +841,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -794,7 +1029,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -806,30 +1065,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -869,9 +1104,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{69278E56-1682-4CF0-8367-FD1CDC3DEE25}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1182,40 +1465,437 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC896E7-E64E-4E8D-9E7F-C6182092A6E8}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:U33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="30.35546875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="49"/>
+    <col min="4" max="4" width="13.140625" style="49" customWidth="1"/>
+    <col min="5" max="16384" width="13.42578125" style="49"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="45.75" customHeight="1">
+      <c r="A1" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+    </row>
+    <row r="2" spans="1:21" ht="14.15">
+      <c r="A2" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="1:21" ht="42.45">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+    </row>
+    <row r="4" spans="1:21" ht="14.15">
+      <c r="A4" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="14.15">
+      <c r="A5" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="1:21" ht="14.15">
+      <c r="A6" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:21" ht="14.15">
+      <c r="A7" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="14.15">
+      <c r="A8" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+    </row>
+    <row r="9" spans="1:21" ht="14.15">
+      <c r="A9" s="61"/>
+      <c r="B9" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="14.15">
+      <c r="A10" s="63"/>
+      <c r="B10" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="14.15">
+      <c r="A11" s="64"/>
+      <c r="B11" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="14.15">
+      <c r="A12" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+    </row>
+    <row r="13" spans="1:21" ht="14.15">
+      <c r="A13" s="61"/>
+      <c r="B13" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="14.15">
+      <c r="A14" s="63"/>
+      <c r="B14" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="14.15">
+      <c r="A15" s="63"/>
+      <c r="B15" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="14.15">
+      <c r="A16" s="63"/>
+      <c r="B16" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.15">
+      <c r="A17" s="64"/>
+      <c r="B17" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.15">
+      <c r="A18" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+    </row>
+    <row r="19" spans="1:4" ht="14.15">
+      <c r="A19" s="61"/>
+      <c r="B19" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.15">
+      <c r="A20" s="63"/>
+      <c r="B20" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.15">
+      <c r="A21" s="64"/>
+      <c r="B21" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.15">
+      <c r="A22" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.15">
+      <c r="A23" s="65"/>
+      <c r="B23" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.15">
+      <c r="A24" s="65"/>
+      <c r="B24" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.15">
+      <c r="A25" s="65"/>
+      <c r="B25" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.15">
+      <c r="A26" s="65"/>
+      <c r="B26" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.15">
+      <c r="A27" s="65"/>
+      <c r="B27" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.15">
+      <c r="A28" s="66"/>
+      <c r="B28" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="12.45">
+      <c r="A29" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="68"/>
+    </row>
+    <row r="30" spans="1:4" ht="12.45">
+      <c r="A30" s="69"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="52"/>
+    </row>
+    <row r="31" spans="1:4" ht="12.9">
+      <c r="A31" s="70"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+    </row>
+    <row r="32" spans="1:4" ht="12.9">
+      <c r="A32" s="70"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+    </row>
+    <row r="33" spans="1:4" ht="12.9">
+      <c r="A33" s="70"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A29:D30"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34E9464-3AEF-074E-A273-00B1548652C2}">
   <dimension ref="B2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15.9"/>
   <cols>
-    <col min="2" max="2" width="4.6484375" customWidth="1"/>
-    <col min="3" max="3" width="31.1484375" customWidth="1"/>
-    <col min="4" max="5" width="17.1484375" customWidth="1"/>
+    <col min="2" max="2" width="4.640625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65"/>
-    <row r="3" spans="2:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B3" s="25" t="s">
+    <row r="2" spans="2:5" ht="16.3" thickBot="1"/>
+    <row r="3" spans="2:5" ht="42" customHeight="1" thickBot="1">
+      <c r="B3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-    </row>
-    <row r="4" spans="2:5" ht="23.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B4" s="23" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="2:5" ht="23.05" customHeight="1" thickBot="1">
+      <c r="B4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="2:5" ht="27.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
+    <row r="5" spans="2:5" ht="28.75" thickBot="1">
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="9" t="s">
         <v>82</v>
       </c>
@@ -1223,51 +1903,51 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B6" s="21" t="s">
+    <row r="6" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="11"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="2:5" ht="17.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B7" s="21" t="s">
+    <row r="7" spans="2:5" ht="17.7" customHeight="1" thickBot="1">
+      <c r="B7" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="11" t="s">
         <v>80</v>
       </c>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B8" s="21" t="s">
+    <row r="8" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B8" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B9" s="21" t="s">
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B9" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B10" s="21" t="s">
+    <row r="10" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B10" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="6"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="2:5" ht="16.3" thickBot="1">
       <c r="B11" s="17"/>
       <c r="C11" s="7" t="s">
         <v>21</v>
@@ -1277,7 +1957,7 @@
       </c>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="2:5" ht="16.3" thickBot="1">
       <c r="B12" s="16"/>
       <c r="C12" s="7" t="s">
         <v>60</v>
@@ -1287,15 +1967,15 @@
       </c>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B13" s="21" t="s">
+    <row r="13" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="6"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="14" spans="2:5" ht="16.3" thickBot="1">
       <c r="B14" s="17"/>
       <c r="C14" s="7" t="s">
         <v>23</v>
@@ -1305,7 +1985,7 @@
       </c>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="2:5" ht="16.3" thickBot="1">
       <c r="B15" s="17"/>
       <c r="C15" s="7" t="s">
         <v>24</v>
@@ -1315,7 +1995,7 @@
       </c>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="2:5" ht="16.3" thickBot="1">
       <c r="B16" s="16"/>
       <c r="C16" s="7" t="s">
         <v>25</v>
@@ -1325,15 +2005,15 @@
       </c>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B17" s="21" t="s">
+    <row r="17" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B17" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="6"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="2:5" ht="16.3" thickBot="1">
       <c r="B18" s="17"/>
       <c r="C18" s="7" t="s">
         <v>27</v>
@@ -1343,7 +2023,7 @@
       </c>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="19" spans="2:5" ht="16.3" thickBot="1">
       <c r="B19" s="17"/>
       <c r="C19" s="7" t="s">
         <v>28</v>
@@ -1353,7 +2033,7 @@
       </c>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="20" spans="2:5" ht="16.3" thickBot="1">
       <c r="B20" s="17"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -1363,7 +2043,7 @@
       </c>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="21" spans="2:5" ht="16.3" thickBot="1">
       <c r="B21" s="17"/>
       <c r="C21" s="7" t="s">
         <v>30</v>
@@ -1373,7 +2053,7 @@
       </c>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="22" spans="2:5" ht="16.3" thickBot="1">
       <c r="B22" s="16"/>
       <c r="C22" s="7" t="s">
         <v>31</v>
@@ -1383,15 +2063,15 @@
       </c>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B23" s="21" t="s">
+    <row r="23" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B23" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="6"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="24" spans="2:5" ht="16.3" thickBot="1">
       <c r="B24" s="17"/>
       <c r="C24" s="7" t="s">
         <v>33</v>
@@ -1401,7 +2081,7 @@
       </c>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="25" spans="2:5" ht="16.3" thickBot="1">
       <c r="B25" s="17"/>
       <c r="C25" s="7" t="s">
         <v>34</v>
@@ -1411,7 +2091,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="26" spans="2:5" ht="16.3" thickBot="1">
       <c r="B26" s="16"/>
       <c r="C26" s="7" t="s">
         <v>35</v>
@@ -1421,15 +2101,15 @@
       </c>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B27" s="21" t="s">
+    <row r="27" spans="2:5" ht="16.3" thickBot="1">
+      <c r="B27" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="6"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="28" spans="2:5" ht="16.3" thickBot="1">
       <c r="B28" s="17"/>
       <c r="C28" s="7" t="s">
         <v>7</v>
@@ -1439,7 +2119,7 @@
       </c>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="29" spans="2:5" ht="16.3" thickBot="1">
       <c r="B29" s="17"/>
       <c r="C29" s="10" t="s">
         <v>9</v>
@@ -1449,7 +2129,7 @@
       </c>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="30" spans="2:5" ht="16.3" thickBot="1">
       <c r="B30" s="17"/>
       <c r="C30" s="7" t="s">
         <v>10</v>
@@ -1459,7 +2139,7 @@
       </c>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="31" spans="2:5" ht="16.3" thickBot="1">
       <c r="B31" s="17"/>
       <c r="C31" s="7" t="s">
         <v>11</v>
@@ -1469,7 +2149,7 @@
       </c>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="32" spans="2:5" ht="16.3" thickBot="1">
       <c r="B32" s="17"/>
       <c r="C32" s="7" t="s">
         <v>12</v>
@@ -1479,7 +2159,7 @@
       </c>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="2:5" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="33" spans="2:5" ht="16.3" thickBot="1">
       <c r="B33" s="18"/>
       <c r="C33" s="19" t="s">
         <v>13</v>
@@ -1491,11 +2171,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B23:C23"/>
@@ -1503,12 +2178,17 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597AAAF1-ECA9-8742-B309-3761F75A3BB5}">
   <dimension ref="B2:I13"/>
   <sheetViews>
@@ -1516,14 +2196,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15.9"/>
   <cols>
     <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="5" max="7" width="17.6484375" customWidth="1"/>
+    <col min="5" max="7" width="17.640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65"/>
-    <row r="3" spans="2:9" ht="26.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:9" ht="16.3" thickBot="1"/>
+    <row r="3" spans="2:9" ht="26.05" customHeight="1" thickBot="1">
       <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
@@ -1534,7 +2214,7 @@
       <c r="G3" s="41"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="2:9" ht="16.3" thickBot="1">
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
@@ -1555,7 +2235,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="2:9" ht="16.3" thickBot="1">
       <c r="B5" s="43"/>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
@@ -1565,7 +2245,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="2:9" ht="24" customHeight="1" thickBot="1">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1587,7 +2267,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="2:9" ht="24" customHeight="1" thickBot="1">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +2289,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="8" spans="2:9" ht="24" customHeight="1" thickBot="1">
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +2311,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="9" spans="2:9" ht="24" customHeight="1" thickBot="1">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1653,7 +2333,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="2:9" ht="24" customHeight="1" thickBot="1">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1675,7 +2355,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="2:9" ht="24" customHeight="1" thickBot="1">
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1697,7 +2377,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="2:9" ht="16.3" thickBot="1">
       <c r="B12" s="33" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +2389,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:9" ht="26.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="13" spans="2:9" ht="26.05" customHeight="1" thickBot="1">
       <c r="B13" s="36" t="s">
         <v>15</v>
       </c>

</xml_diff>